<commit_message>
adding checks and fixing error of brachot starting page of chapter 7
</commit_message>
<xml_diff>
--- a/src/bavli_pages/all_pages.xlsx
+++ b/src/bavli_pages/all_pages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reut\Documents\lior\python\my_pypi_packages\bavli_pages\src\bavli_pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\israelil\Downloads\my_things\pypi\bavli_pages\src\bavli_pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB59A13-E5DE-44C4-AA9F-6292990A318C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F77B7F-8F67-4093-B244-B6A1472AD7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EBE44150-A838-439B-83AA-F0B42107DC3F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EBE44150-A838-439B-83AA-F0B42107DC3F}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -989,7 +989,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1287,16 +1287,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C2167B-5345-4EBF-890C-D3D712ABB1C0}">
   <dimension ref="A1:AW38"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="3.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1445,7 +1442,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -1489,7 +1486,7 @@
         <v>66</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>68</v>
@@ -1534,7 +1531,7 @@
       <c r="AV2" s="1"/>
       <c r="AW2" s="1"/>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>72</v>
       </c>
@@ -1683,7 +1680,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>100</v>
       </c>
@@ -1776,7 +1773,7 @@
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>105</v>
       </c>
@@ -1869,7 +1866,7 @@
       <c r="AV5" s="1"/>
       <c r="AW5" s="1"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>120</v>
       </c>
@@ -1954,7 +1951,7 @@
       <c r="AV6" s="1"/>
       <c r="AW6" s="1"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>130</v>
       </c>
@@ -2027,7 +2024,7 @@
       <c r="AV7" s="1"/>
       <c r="AW7" s="1"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>133</v>
       </c>
@@ -2100,7 +2097,7 @@
       <c r="AV8" s="1"/>
       <c r="AW8" s="1"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>139</v>
       </c>
@@ -2169,7 +2166,7 @@
       <c r="AV9" s="1"/>
       <c r="AW9" s="1"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>141</v>
       </c>
@@ -2238,7 +2235,7 @@
       <c r="AV10" s="1"/>
       <c r="AW10" s="1"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>144</v>
       </c>
@@ -2307,7 +2304,7 @@
       <c r="AV11" s="1"/>
       <c r="AW11" s="1"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>147</v>
       </c>
@@ -2372,7 +2369,7 @@
       <c r="AV12" s="1"/>
       <c r="AW12" s="1"/>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>152</v>
       </c>
@@ -2437,7 +2434,7 @@
       <c r="AV13" s="1"/>
       <c r="AW13" s="1"/>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>154</v>
       </c>
@@ -2554,7 +2551,7 @@
       <c r="AV14" s="1"/>
       <c r="AW14" s="1"/>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>166</v>
       </c>
@@ -2659,7 +2656,7 @@
       <c r="AV15" s="1"/>
       <c r="AW15" s="1"/>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>177</v>
       </c>
@@ -2756,7 +2753,7 @@
       <c r="AV16" s="1"/>
       <c r="AW16" s="1"/>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>187</v>
       </c>
@@ -2845,7 +2842,7 @@
       <c r="AV17" s="1"/>
       <c r="AW17" s="1"/>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>192</v>
       </c>
@@ -2934,7 +2931,7 @@
       <c r="AV18" s="1"/>
       <c r="AW18" s="1"/>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>198</v>
       </c>
@@ -3023,7 +3020,7 @@
       <c r="AV19" s="1"/>
       <c r="AW19" s="1"/>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>202</v>
       </c>
@@ -3092,7 +3089,7 @@
       <c r="AV20" s="1"/>
       <c r="AW20" s="1"/>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>206</v>
       </c>
@@ -3185,7 +3182,7 @@
       <c r="AV21" s="1"/>
       <c r="AW21" s="1"/>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>215</v>
       </c>
@@ -3278,7 +3275,7 @@
       <c r="AV22" s="1"/>
       <c r="AW22" s="1"/>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>224</v>
       </c>
@@ -3371,7 +3368,7 @@
       <c r="AV23" s="1"/>
       <c r="AW23" s="1"/>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>232</v>
       </c>
@@ -3468,7 +3465,7 @@
       <c r="AV24" s="1"/>
       <c r="AW24" s="1"/>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>242</v>
       </c>
@@ -3533,7 +3530,7 @@
       <c r="AV25" s="1"/>
       <c r="AW25" s="1"/>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>245</v>
       </c>
@@ -3618,7 +3615,7 @@
       <c r="AV26" s="1"/>
       <c r="AW26" s="1"/>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>248</v>
       </c>
@@ -3691,7 +3688,7 @@
       <c r="AV27" s="1"/>
       <c r="AW27" s="1"/>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>249</v>
       </c>
@@ -3756,7 +3753,7 @@
       <c r="AV28" s="1"/>
       <c r="AW28" s="1"/>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>252</v>
       </c>
@@ -3865,7 +3862,7 @@
       <c r="AV29" s="1"/>
       <c r="AW29" s="1"/>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>259</v>
       </c>
@@ -3970,7 +3967,7 @@
       <c r="AV30" s="1"/>
       <c r="AW30" s="1"/>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>264</v>
       </c>
@@ -4071,7 +4068,7 @@
       <c r="AV31" s="1"/>
       <c r="AW31" s="1"/>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>272</v>
       </c>
@@ -4160,7 +4157,7 @@
       <c r="AV32" s="1"/>
       <c r="AW32" s="1"/>
     </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>273</v>
       </c>
@@ -4249,7 +4246,7 @@
       <c r="AV33" s="1"/>
       <c r="AW33" s="1"/>
     </row>
-    <row r="34" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>275</v>
       </c>
@@ -4330,7 +4327,7 @@
       <c r="AV34" s="1"/>
       <c r="AW34" s="1"/>
     </row>
-    <row r="35" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>276</v>
       </c>
@@ -4407,7 +4404,7 @@
       <c r="AV35" s="1"/>
       <c r="AW35" s="1"/>
     </row>
-    <row r="36" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>277</v>
       </c>
@@ -4484,7 +4481,7 @@
       <c r="AV36" s="1"/>
       <c r="AW36" s="1"/>
     </row>
-    <row r="37" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>282</v>
       </c>
@@ -4565,7 +4562,7 @@
       <c r="AV37" s="1"/>
       <c r="AW37" s="1"/>
     </row>
-    <row r="38" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>284</v>
       </c>
@@ -4661,5 +4658,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>